<commit_message>
>  compile NEMU MyonieOs Myonie Linux myonie-virtual-machine 5.19.0-35-generic #36~22.04.1-Ubuntu SMP PREEMPT_DYNAMIC Fri Feb 17 15:17:25 UTC 2 x86_64 x86_64 x86_64 GNU/Linux  20:50:11 up 1 day, 19:35,  1 user,  load average: 1.31, 0.48, 0.27
</commit_message>
<xml_diff>
--- a/docs/RV64MC-Instr.xlsx
+++ b/docs/RV64MC-Instr.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -426,6 +426,9 @@
       <c r="K2" t="str">
         <v>V</v>
       </c>
+      <c r="N2" t="str">
+        <v>OPSET</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -468,6 +471,9 @@
       <c r="J5" t="str">
         <v>funct6</v>
       </c>
+      <c r="N5" t="str">
+        <v>funct6</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -547,9 +553,24 @@
         <v>mld</v>
       </c>
     </row>
+    <row r="9">
+      <c r="E9" t="str">
+        <v>000011</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="E10" t="str">
+        <v>000100</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="E11" t="str">
+        <v>000101</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
>  compile NEMU MyonieOs Myonie Linux myonie-virtual-machine 5.19.0-41-generic #42~22.04.1-Ubuntu SMP PREEMPT_DYNAMIC Tue Apr 18 17:40:00 UTC 2 x86_64 x86_64 x86_64 GNU/Linux  16:32:00 up 19:13,  1 user,  load average: 0.52, 0.36, 0.36
</commit_message>
<xml_diff>
--- a/docs/RV64MC-Instr.xlsx
+++ b/docs/RV64MC-Instr.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -637,10 +637,10 @@
         <v>000101</v>
       </c>
       <c r="O12" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" t="str">
         <v>X</v>
@@ -665,10 +665,10 @@
     </row>
     <row r="14">
       <c r="O14" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14" t="str">
         <v>X</v>
@@ -693,10 +693,10 @@
     </row>
     <row r="16">
       <c r="O16" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q16" t="str">
         <v>X</v>
@@ -721,18 +721,43 @@
     </row>
     <row r="18">
       <c r="O18" t="str">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" t="str">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="str">
+        <v>X</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="N19" t="str">
+        <v>0101</v>
+      </c>
+      <c r="O19" t="str">
+        <v>0</v>
+      </c>
+      <c r="P19" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="str">
+        <v>I</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="O20" t="str">
+        <v>1</v>
+      </c>
+      <c r="P20" t="str">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="str">
         <v>X</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>